<commit_message>
REPORTGEN-508 : adjust column size in new template
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting/TemplatesFiles/AEP-sample-Template.xlsx
+++ b/CastReporting.Reporting/TemplatesFiles/AEP-sample-Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\1.9\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDCB970-82C3-41F8-9C34-D854B56EF04F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5960A8F-A872-4A85-BF8F-DA9BEC6342C3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -1263,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -1379,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1387,8 +1387,11 @@
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="8" width="19.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
@@ -1472,8 +1475,9 @@
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="7" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>
@@ -1551,15 +1555,15 @@
   <dimension ref="B1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
     <col min="11" max="11" width="14.28515625" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" customWidth="1"/>

</xml_diff>